<commit_message>
player fire change to FireinFan
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/player_parameter.xlsx
+++ b/Engine/data/datasheet/player_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B70E93-CCCC-4E1B-81BD-B90C9E639212}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9556D5-1827-4CB4-A13F-8A0F09B145C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="2190" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A7" sqref="A7:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
balace and player reload added
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/player_parameter.xlsx
+++ b/Engine/data/datasheet/player_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F4D9A5-0075-4C9D-B288-2EE98CF97DC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BEAB35-9E73-4836-8AC4-3D7F3BCB06C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1122,7 +1122,7 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>

</xml_diff>